<commit_message>
Se agrego Alertas por piezay se inserto en el formulario de devolución la penalización.
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5FC4B9-581B-4B79-8734-EE43ADAB04B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F0F124-109E-4408-AB08-0AD6F67F0BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -172,7 +172,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +185,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,21 +231,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -563,50 +592,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AR9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AO11" sqref="AO11"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AO9" sqref="AO9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
@@ -615,150 +650,150 @@
       </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Y8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="Z8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AB8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AC8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AE8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AF8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AG8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AH8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AI8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AJ8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AK8" s="1" t="s">
+      <c r="AK8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AL8" s="1" t="s">
+      <c r="AL8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AM8" s="1" t="s">
+      <c r="AM8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AN8" s="1" t="s">
+      <c r="AN8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AO8" s="1" t="s">
+      <c r="AO8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AP8" s="1" t="s">
+      <c r="AP8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AQ8" s="1" t="s">
+      <c r="AQ8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AR8" s="1" t="s">
+      <c r="AR8" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generar excel utilidad bruta
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F0F124-109E-4408-AB08-0AD6F67F0BD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0E699-E2A0-4627-AD87-69FD35C73933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Fecha:</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>UTILIDAD FINAL</t>
+  </si>
+  <si>
+    <t>SUB TOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>UTILIDAD BRUTA</t>
   </si>
 </sst>
 </file>
@@ -249,9 +258,6 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -259,6 +265,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -590,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AR9"/>
+  <dimension ref="A2:AU9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AO9" sqref="AO9"/>
+      <selection activeCell="AR12" sqref="AR12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,158 +650,170 @@
     <col min="41" max="41" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="K2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="F3" s="5" t="s">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="F3" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="O8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="P8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="R8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="S8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="T8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U8" s="6" t="s">
+      <c r="U8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V8" s="6" t="s">
+      <c r="V8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="W8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="X8" s="6" t="s">
+      <c r="X8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y8" s="6" t="s">
+      <c r="Y8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Z8" s="6" t="s">
+      <c r="Z8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA8" s="6" t="s">
+      <c r="AA8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="6" t="s">
+      <c r="AB8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AC8" s="6" t="s">
+      <c r="AC8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AD8" s="6" t="s">
+      <c r="AD8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AE8" s="8" t="s">
+      <c r="AE8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="6" t="s">
+      <c r="AF8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AG8" s="6" t="s">
+      <c r="AG8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AH8" s="6" t="s">
+      <c r="AH8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AI8" s="6" t="s">
+      <c r="AI8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AJ8" s="6" t="s">
+      <c r="AJ8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AK8" s="6" t="s">
+      <c r="AK8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AL8" s="7" t="s">
+      <c r="AL8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AM8" s="7" t="s">
+      <c r="AM8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AN8" s="6" t="s">
+      <c r="AN8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AO8" s="6" t="s">
+      <c r="AO8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AP8" s="7" t="s">
+      <c r="AP8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AQ8" s="7" t="s">
+      <c r="AT8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AR8" s="7" t="s">
+      <c r="AU8" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Diseño a formularios y se modifico la consulta para generar el excel.
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D0E699-E2A0-4627-AD87-69FD35C73933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD02A7A6-ABD2-4BFC-A5D5-887E0FD9CF33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Fecha:</t>
   </si>
@@ -54,18 +54,12 @@
     <t>PROVEEDOR</t>
   </si>
   <si>
-    <t>PIEZA</t>
-  </si>
-  <si>
     <t>CLAVE PRODUCTO</t>
   </si>
   <si>
     <t>TOTAL DE PIEZAS</t>
   </si>
   <si>
-    <t>GUÍA DE SEGUIMIENTO</t>
-  </si>
-  <si>
     <t>ORIGEN PIEZA</t>
   </si>
   <si>
@@ -75,12 +69,6 @@
     <t>COSTO ENVÍO</t>
   </si>
   <si>
-    <t>COSTO SIN IVA</t>
-  </si>
-  <si>
-    <t>COSTO CON IVA</t>
-  </si>
-  <si>
     <t>PRECIO VENTA</t>
   </si>
   <si>
@@ -162,29 +150,39 @@
     <t>COSTO OPERATIVO</t>
   </si>
   <si>
-    <t>TOTAL GASTO</t>
-  </si>
-  <si>
     <t>UTILIDAD FINAL</t>
   </si>
   <si>
-    <t>SUB TOTAL</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>UTILIDAD BRUTA</t>
+    <t>PIEZAS</t>
+  </si>
+  <si>
+    <t>GUÍA DE ENVIO</t>
+  </si>
+  <si>
+    <t>COSTO</t>
+  </si>
+  <si>
+    <t>COSTO ADQUISICION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTILIDAD ADQUISICION </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GASTO</t>
+  </si>
+  <si>
+    <t>MARCA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,13 +205,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -240,11 +252,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,20 +271,24 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -599,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AU9"/>
+  <dimension ref="A2:AT9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AR12" sqref="AR12"/>
+      <selection activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,17 +630,17 @@
     <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="1"/>
     <col min="20" max="20" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -648,29 +665,29 @@
     <col min="39" max="39" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="24.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="K2" s="2" t="s">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -690,137 +707,134 @@
         <v>6</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="M8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="O8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="P8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="Q8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="S8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="6" t="s">
+      <c r="T8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="U8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="V8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="5" t="s">
+      <c r="X8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="Y8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="Z8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W8" s="5" t="s">
+      <c r="AA8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="X8" s="5" t="s">
+      <c r="AB8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y8" s="5" t="s">
+      <c r="AC8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Z8" s="5" t="s">
+      <c r="AD8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA8" s="5" t="s">
+      <c r="AE8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="5" t="s">
+      <c r="AF8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AC8" s="5" t="s">
+      <c r="AG8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AD8" s="5" t="s">
+      <c r="AH8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AE8" s="7" t="s">
+      <c r="AI8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AF8" s="5" t="s">
+      <c r="AJ8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AG8" s="5" t="s">
+      <c r="AK8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AH8" s="5" t="s">
+      <c r="AL8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AI8" s="5" t="s">
+      <c r="AM8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ8" s="5" t="s">
+      <c r="AN8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AK8" s="5" t="s">
+      <c r="AO8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AL8" s="6" t="s">
+      <c r="AP8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT8" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AM8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU8" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Diseño de formulario y arreglo de algunos querys.
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -8,17 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD02A7A6-ABD2-4BFC-A5D5-887E0FD9CF33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CF7C39-9B0D-4797-8674-5C44EBB1D2F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,9 +53,6 @@
     <t>TALLER</t>
   </si>
   <si>
-    <t>VHEICULO MODELO</t>
-  </si>
-  <si>
     <t>AÑO</t>
   </si>
   <si>
@@ -172,6 +177,9 @@
   </si>
   <si>
     <t>MARCA</t>
+  </si>
+  <si>
+    <t>VEHICULO MODELO</t>
   </si>
 </sst>
 </file>
@@ -618,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AT9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AO8" sqref="AO8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +687,7 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="F3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -704,132 +712,132 @@
         <v>5</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="L8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="O8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="P8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="S8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AP8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="U8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="W8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="X8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP8" s="6" t="s">
+      <c r="AQ8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AQ8" s="6" t="s">
+      <c r="AR8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AR8" s="6" t="s">
+      <c r="AT8" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="AS8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT8" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
diseño y arreglo bugs
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CF7C39-9B0D-4797-8674-5C44EBB1D2F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E00856D-4417-4E50-956B-71E81C504870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Fecha:</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>VEHICULO MODELO</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -259,13 +262,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -294,6 +310,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -624,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AT9"/>
+  <dimension ref="A2:AU9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="AL8" workbookViewId="0">
+      <selection activeCell="AU14" sqref="AU14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,12 +703,12 @@
     <col min="46" max="46" width="15" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="F3" s="9" t="s">
         <v>38</v>
       </c>
@@ -695,7 +718,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -831,14 +854,18 @@
       <c r="AS8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AT8" s="6" t="s">
+      <c r="AT8" s="10" t="s">
         <v>40</v>
       </c>
+      <c r="AU8" s="11" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="AU9" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se añadieron validaciones a los formularios Bryan y se modificó el excel.
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E00856D-4417-4E50-956B-71E81C504870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EC40F5-B895-4DD2-8624-FA6100AFC816}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>VEHICULO MODELO</t>
   </si>
   <si>
-    <t>.</t>
+    <t>NUMERO DE VENDEDOR</t>
   </si>
 </sst>
 </file>
@@ -281,7 +281,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -307,16 +307,13 @@
     <xf numFmtId="44" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -650,7 +647,7 @@
   <dimension ref="A2:AU9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AL8" workbookViewId="0">
-      <selection activeCell="AU14" sqref="AU14"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +671,7 @@
     <col min="17" max="17" width="14.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="1"/>
-    <col min="20" max="20" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -701,6 +698,7 @@
     <col min="44" max="44" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:47" x14ac:dyDescent="0.25">
@@ -709,14 +707,14 @@
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -777,95 +775,95 @@
         <v>14</v>
       </c>
       <c r="T8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="U8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U8" s="5" t="s">
+      <c r="V8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="W8" s="5" t="s">
+      <c r="X8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="X8" s="5" t="s">
+      <c r="Y8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Y8" s="5" t="s">
+      <c r="Z8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="Z8" s="5" t="s">
+      <c r="AA8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AA8" s="5" t="s">
+      <c r="AB8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AB8" s="5" t="s">
+      <c r="AC8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AC8" s="5" t="s">
+      <c r="AD8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AD8" s="5" t="s">
+      <c r="AE8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AE8" s="7" t="s">
+      <c r="AF8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AF8" s="5" t="s">
+      <c r="AG8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AG8" s="5" t="s">
+      <c r="AH8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AH8" s="5" t="s">
+      <c r="AI8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AI8" s="5" t="s">
+      <c r="AJ8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AJ8" s="5" t="s">
+      <c r="AK8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AK8" s="5" t="s">
+      <c r="AL8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AL8" s="6" t="s">
+      <c r="AM8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AM8" s="6" t="s">
+      <c r="AN8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AN8" s="5" t="s">
+      <c r="AO8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AP8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AP8" s="6" t="s">
+      <c r="AQ8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AQ8" s="6" t="s">
+      <c r="AR8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AR8" s="6" t="s">
+      <c r="AS8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AS8" s="8" t="s">
+      <c r="AT8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AT8" s="10" t="s">
+      <c r="AU8" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="AU8" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AU9" s="12"/>
+      <c r="AU9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Arreglo bugs al exportar excel
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\proyectoJeic\Jeic\Axdrox\proyectoJeic\Jeic\Jeic\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10E112D-59C6-4D9C-BA26-7EC1199AA348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33781C11-CF38-4019-A204-230CB3A645D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Fecha:</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>NUMERO DE VENDEDOR</t>
+  </si>
+  <si>
+    <t>PIEZAS DEVUELTAS ANTES DE ENTREGA</t>
   </si>
 </sst>
 </file>
@@ -311,10 +314,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,79 +650,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AU9"/>
+  <dimension ref="A2:AV9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="6" max="6" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="1"/>
+    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="1"/>
+    <col min="19" max="19" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="31.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="15" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="F3" s="11" t="s">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="F3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -817,52 +821,55 @@
         <v>26</v>
       </c>
       <c r="AG8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AH8" s="4" t="s">
+      <c r="AI8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AI8" s="4" t="s">
+      <c r="AJ8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AJ8" s="4" t="s">
+      <c r="AK8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AK8" s="4" t="s">
+      <c r="AL8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AL8" s="4" t="s">
+      <c r="AM8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AM8" s="8" t="s">
+      <c r="AN8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AN8" s="8" t="s">
+      <c r="AO8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AO8" s="4" t="s">
+      <c r="AP8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AP8" s="4" t="s">
+      <c r="AQ8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AQ8" s="5" t="s">
+      <c r="AR8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AR8" s="8" t="s">
+      <c r="AS8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AS8" s="8" t="s">
+      <c r="AT8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AT8" s="9" t="s">
+      <c r="AU8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AU8" s="10" t="s">
+      <c r="AV8" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Agregaron datos al EXCEL y se modificó administrar
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33781C11-CF38-4019-A204-230CB3A645D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB777D9C-B2E1-4D5E-914E-60023D8561E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Fecha:</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>PIEZAS DEVUELTAS ANTES DE ENTREGA</t>
+  </si>
+  <si>
+    <t>DESCRIPCION APLICACIÓN SAE</t>
   </si>
 </sst>
 </file>
@@ -650,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AV9"/>
+  <dimension ref="A2:AW9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,51 +672,52 @@
     <col min="9" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="F3" s="12" t="s">
         <v>38</v>
       </c>
@@ -723,7 +727,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -758,118 +762,121 @@
         <v>8</v>
       </c>
       <c r="L8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="Q8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="R8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="S8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="U8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="V8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="V8" s="4" t="s">
+      <c r="W8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="X8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="X8" s="4" t="s">
+      <c r="Y8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="Z8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Z8" s="4" t="s">
+      <c r="AA8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AA8" s="4" t="s">
+      <c r="AB8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AB8" s="4" t="s">
+      <c r="AC8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AC8" s="4" t="s">
+      <c r="AD8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AD8" s="4" t="s">
+      <c r="AE8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AE8" s="8" t="s">
+      <c r="AF8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AF8" s="7" t="s">
+      <c r="AG8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AG8" s="4" t="s">
+      <c r="AH8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AH8" s="4" t="s">
+      <c r="AI8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AI8" s="4" t="s">
+      <c r="AJ8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AJ8" s="4" t="s">
+      <c r="AK8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK8" s="4" t="s">
+      <c r="AL8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AL8" s="4" t="s">
+      <c r="AM8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AM8" s="4" t="s">
+      <c r="AN8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AN8" s="8" t="s">
+      <c r="AO8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AO8" s="8" t="s">
+      <c r="AP8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AP8" s="4" t="s">
+      <c r="AQ8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AQ8" s="4" t="s">
+      <c r="AR8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AR8" s="5" t="s">
+      <c r="AS8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AS8" s="8" t="s">
+      <c r="AT8" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AT8" s="8" t="s">
+      <c r="AU8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AU8" s="9" t="s">
+      <c r="AV8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AV8" s="10" t="s">
+      <c r="AW8" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Se agregó lo solicitado al Excel
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB777D9C-B2E1-4D5E-914E-60023D8561E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C846C6-B9BE-48FC-9279-2C87D6FD327A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Fecha:</t>
   </si>
@@ -113,9 +113,6 @@
     <t>CANTIDAD DE PIEZAS DEVUELTAS</t>
   </si>
   <si>
-    <t>PENALIZACIÓN POR DEVOLUCIÓN</t>
-  </si>
-  <si>
     <t>FACTURA ACTUAL</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>DESCRIPCION APLICACIÓN SAE</t>
+  </si>
+  <si>
+    <t>PENALIZACIÓN POR DEVOLUCIÓN (%)</t>
+  </si>
+  <si>
+    <t>PENALIZACIÓN POR DEVOLUCIÓN ANTES DE ENTREGA (%)</t>
   </si>
 </sst>
 </file>
@@ -653,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AW9"/>
+  <dimension ref="A2:AX9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG9" sqref="AG9"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,33 +696,34 @@
     <col min="30" max="30" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="24" style="11" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="31.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="18" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="53" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="F3" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -727,7 +731,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -744,10 +748,10 @@
         <v>5</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>6</v>
@@ -756,19 +760,19 @@
         <v>7</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>10</v>
@@ -780,7 +784,7 @@
         <v>12</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>13</v>
@@ -789,7 +793,7 @@
         <v>14</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V8" s="4" t="s">
         <v>15</v>
@@ -825,62 +829,65 @@
         <v>25</v>
       </c>
       <c r="AG8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AH8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AI8" s="4" t="s">
+      <c r="AK8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AJ8" s="4" t="s">
+      <c r="AL8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AK8" s="4" t="s">
+      <c r="AM8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AL8" s="4" t="s">
+      <c r="AN8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AM8" s="4" t="s">
+      <c r="AO8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AN8" s="4" t="s">
+      <c r="AP8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AO8" s="8" t="s">
+      <c r="AQ8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AP8" s="8" t="s">
+      <c r="AR8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AQ8" s="4" t="s">
+      <c r="AS8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AR8" s="4" t="s">
+      <c r="AT8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AX8" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AS8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU8" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW8" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Versión 1.1.8 con algunos pequeños cambios en el excel se agregó estado a la hora de exportar
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C846C6-B9BE-48FC-9279-2C87D6FD327A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AF6BC0-E312-4A55-A413-83B22FC4A126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Fecha:</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>PENALIZACIÓN POR DEVOLUCIÓN ANTES DE ENTREGA (%)</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AX9"/>
+  <dimension ref="A2:AY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AS8" sqref="AS8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,20 +711,19 @@
     <col min="42" max="42" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="18" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="F3" s="12" t="s">
         <v>37</v>
       </c>
@@ -731,7 +733,7 @@
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -865,25 +867,28 @@
         <v>34</v>
       </c>
       <c r="AS8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AT8" s="5" t="s">
+      <c r="AU8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AU8" s="8" t="s">
+      <c r="AV8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AV8" s="8" t="s">
+      <c r="AW8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AW8" s="9" t="s">
+      <c r="AX8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AX8" s="10" t="s">
+      <c r="AY8" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Versión 2.0.1 Lita bugs fixed!
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BuGsBunNy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AF6BC0-E312-4A55-A413-83B22FC4A126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE05E441-4438-4468-A95A-E662E6F72A73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AY9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AS8" sqref="AS8"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +695,7 @@
     <col min="26" max="26" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="24" style="11" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="30.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -807,7 +807,7 @@
         <v>17</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>19</v>
@@ -819,7 +819,7 @@
         <v>21</v>
       </c>
       <c r="AC8" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AD8" s="4" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Version 2.0.9.9 cveGuia con lector
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81752B82-BBDA-4598-83F5-15FA647E1F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9004929-A9EF-4245-AAE0-181BBA0ADED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Fecha:</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>ESTADO</t>
+  </si>
+  <si>
+    <t>UBICACIÓN</t>
   </si>
 </sst>
 </file>
@@ -322,10 +325,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AY9"/>
+  <dimension ref="A2:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AV13" sqref="AV13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,25 +718,26 @@
     <col min="48" max="48" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="51" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="16384" width="8.88671875" style="1"/>
+    <col min="52" max="52" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="L2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="F3" s="10" t="s">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="F3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
-    <row r="8" spans="1:51" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -887,8 +891,11 @@
       <c r="AY8" s="8" t="s">
         <v>39</v>
       </c>
+      <c r="AZ8" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Version 2.1.6.0 se agrego columna chofer al generar reporte de ventas
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9004929-A9EF-4245-AAE0-181BBA0ADED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94312EB-6D07-40EE-B37E-E89B0F1E1C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Fecha:</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>UBICACIÓN</t>
+  </si>
+  <si>
+    <t>CHOFER</t>
   </si>
 </sst>
 </file>
@@ -661,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AZ9"/>
+  <dimension ref="A2:BA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AV13" sqref="AV13"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AT11" sqref="AT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -713,21 +716,22 @@
     <col min="42" max="42" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="8.88671875" style="1"/>
+    <col min="45" max="45" width="24.33203125" style="2" customWidth="1"/>
+    <col min="46" max="47" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
       <c r="L2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
       <c r="F3" s="11" t="s">
         <v>37</v>
       </c>
@@ -737,7 +741,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="8" spans="1:52" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -894,8 +898,11 @@
       <c r="AZ8" s="8" t="s">
         <v>54</v>
       </c>
+      <c r="BA8" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Version 2.1.7.0 se agrego la columna valeLiberado, se actualiza en automatico cuando se marca la baja de la pieza y se valido que solo se puedan facturar piezas que tengan el estado de ENTREGADO, se eliminaron algunos estados de pedido y se cambiaron reglas al generar el EXCEL.
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/bin/Debug/Plantilla.xlsx
+++ b/Jeic/Jeic/bin/Debug/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94312EB-6D07-40EE-B37E-E89B0F1E1C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5AD2A9-C123-422E-95DE-066AD78111AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Fecha:</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>CHOFER</t>
+  </si>
+  <si>
+    <t>ESTADO DEL VALE</t>
   </si>
 </sst>
 </file>
@@ -664,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:BA9"/>
+  <dimension ref="A2:BB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AT11" sqref="AT11"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BB8" sqref="BB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,15 +726,16 @@
     <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.88671875" style="1"/>
+    <col min="54" max="54" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="L2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.3">
       <c r="F3" s="11" t="s">
         <v>37</v>
       </c>
@@ -741,7 +745,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="8" spans="1:53" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>1</v>
       </c>
@@ -901,8 +905,11 @@
       <c r="BA8" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="BB8" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>

</xml_diff>